<commit_message>
fix set link image in excel into database
</commit_message>
<xml_diff>
--- a/data/lastVersion.xlsx
+++ b/data/lastVersion.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>شماره ردیف</t>
   </si>
@@ -65,367 +65,6 @@
   </si>
   <si>
     <t>آیا این زمان تکمیل شده است؟</t>
-  </si>
-  <si>
-    <t>اکبر</t>
-  </si>
-  <si>
-    <t>یوسفی</t>
-  </si>
-  <si>
-    <t>مهندسی برق</t>
-  </si>
-  <si>
-    <t>قدرت</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>@golam</t>
-  </si>
-  <si>
-    <t>https://ece.ut.ac.ir/image/edu/teacher?img_id=71874335&amp;t=1585488639782</t>
-  </si>
-  <si>
-    <t>پسر خوبیه هستند</t>
-  </si>
-  <si>
-    <t>شنبه ها بعد از ظهر</t>
-  </si>
-  <si>
-    <t>حسن</t>
-  </si>
-  <si>
-    <t>اوقلی</t>
-  </si>
-  <si>
-    <t>مهندسی کامپیوتر</t>
-  </si>
-  <si>
-    <t>هوش مصنوعی</t>
-  </si>
-  <si>
-    <t>4321</t>
-  </si>
-  <si>
-    <t>@ali</t>
-  </si>
-  <si>
-    <t>استاد بدی نیست</t>
-  </si>
-  <si>
-    <t>شنبه ها</t>
-  </si>
-  <si>
-    <t>دوشنب ها</t>
-  </si>
-  <si>
-    <t>علی</t>
-  </si>
-  <si>
-    <t>فرامرزی</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>اسکایپ</t>
-  </si>
-  <si>
-    <t>http://www.talab.org/wp-content/uploads/2017/05/1214775883-talab-org.jpg</t>
-  </si>
-  <si>
-    <t>مهندس خفن</t>
-  </si>
-  <si>
-    <t>یک شنبه ساعت 5 تا 8</t>
-  </si>
-  <si>
-    <t>دوشنبه</t>
-  </si>
-  <si>
-    <t>دوشنبه ساعت 6</t>
-  </si>
-  <si>
-    <t>سه شنبه</t>
-  </si>
-  <si>
-    <t>حسنی</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>زنگ بزن</t>
-  </si>
-  <si>
-    <t>https://wikichejoor.ir/wp-content/uploads/2016/11/3-19.jpg</t>
-  </si>
-  <si>
-    <t>استاد قوی</t>
-  </si>
-  <si>
-    <t>شنبه</t>
-  </si>
-  <si>
-    <t>یکشنبه</t>
-  </si>
-  <si>
-    <t>علیرضا</t>
-  </si>
-  <si>
-    <t>باقری</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>برای هماهنگی قطعی شدن زمان به ایمیل alireza.bagheri.sh@gmail.com پیام بدهید.</t>
-  </si>
-  <si>
-    <t>http://uplod.ir/1u2rkn6hpaka/ali_bagheri.JPG.htm</t>
-  </si>
-  <si>
-    <t>محمد</t>
-  </si>
-  <si>
-    <t>فتحی</t>
-  </si>
-  <si>
-    <t>مهندسی مکانیک</t>
-  </si>
-  <si>
-    <t>تبدیل انرژی</t>
-  </si>
-  <si>
-    <t>201</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>http://s11.picofile.com/file/8392736500/fathi.JPG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">مصطفی </t>
-  </si>
-  <si>
-    <t>الوندیان</t>
-  </si>
-  <si>
-    <t>مخابرات</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>هماهنگی و تماس از طریق واتساپ و با 09212405364</t>
-  </si>
-  <si>
-    <t>http://s10.picofile.com/file/8392736442/alvandian.JPG</t>
-  </si>
-  <si>
-    <t>ایوب</t>
-  </si>
-  <si>
-    <t>طراحی کاربردی</t>
-  </si>
-  <si>
-    <t>202</t>
-  </si>
-  <si>
-    <t>http://s10.picofile.com/file/8392736450/ayoub_hasani.JPG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">محمدرضا </t>
-  </si>
-  <si>
-    <t>فرحناک</t>
-  </si>
-  <si>
-    <t>203</t>
-  </si>
-  <si>
-    <t>http://s11.picofile.com/file/8392736484/farahnak.JPG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">علیرضا </t>
-  </si>
-  <si>
-    <t>قادری</t>
-  </si>
-  <si>
-    <t>مهندسی نفت</t>
-  </si>
-  <si>
-    <t>مخازن هیدروکربوری</t>
-  </si>
-  <si>
-    <t>701</t>
-  </si>
-  <si>
-    <t>http://s10.picofile.com/file/8392736526/ghaderi.JPG</t>
-  </si>
-  <si>
-    <t>محسن</t>
-  </si>
-  <si>
-    <t>غلامی</t>
-  </si>
-  <si>
-    <t>204</t>
-  </si>
-  <si>
-    <t>http://s11.picofile.com/file/8392736550/gholami.JPG</t>
-  </si>
-  <si>
-    <t>رمضان</t>
-  </si>
-  <si>
-    <t>حسینی</t>
-  </si>
-  <si>
-    <t>205</t>
-  </si>
-  <si>
-    <t>http://s11.picofile.com/file/8392736592/hoseini.JPG</t>
-  </si>
-  <si>
-    <t>سعید</t>
-  </si>
-  <si>
-    <t>جلیلوند</t>
-  </si>
-  <si>
-    <t>206</t>
-  </si>
-  <si>
-    <t>http://s11.picofile.com/file/8392736626/jalilvand.JPG</t>
-  </si>
-  <si>
-    <t>سیدحسین</t>
-  </si>
-  <si>
-    <t>کمالی</t>
-  </si>
-  <si>
-    <t>207</t>
-  </si>
-  <si>
-    <t>http://s11.picofile.com/file/8392741392/kamali.JPG</t>
-  </si>
-  <si>
-    <t>جمال</t>
-  </si>
-  <si>
-    <t>کزازی</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>تماس از طریق تلفن یا تلگرام با شماره 9187042184</t>
-  </si>
-  <si>
-    <t>http://s10.picofile.com/file/8392736976/kazzazi.JPG</t>
-  </si>
-  <si>
-    <t>کورش</t>
-  </si>
-  <si>
-    <t>خلج مفرد</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">هماهنگی و تماس از طریق تلگرام با ایدی @Kkmonfared و همچنین تماس از طریق اسکایپ با شماره 9128303218
-</t>
-  </si>
-  <si>
-    <t>http://s10.picofile.com/file/8392736684/khalaj.JPG</t>
-  </si>
-  <si>
-    <t>سیدمیلاد</t>
-  </si>
-  <si>
-    <t>میری</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>هماهنگی و تماس صوتی با تلفن همراه یا تماس از طریق واتساپ از طریق شماره 09117716042</t>
-  </si>
-  <si>
-    <t>http://s11.picofile.com/file/8392736718/miri.JPG</t>
-  </si>
-  <si>
-    <t>امیر</t>
-  </si>
-  <si>
-    <t>ملایی</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>هماهنگی و تماس با تلفن همراه از طریق شماره 9157131289</t>
-  </si>
-  <si>
-    <t>http://s10.picofile.com/file/8392736726/mollaii.JPG</t>
-  </si>
-  <si>
-    <t>حسین</t>
-  </si>
-  <si>
-    <t>208</t>
-  </si>
-  <si>
-    <t>http://s11.picofile.com/file/8392736742/saeed_hosein.JPG</t>
-  </si>
-  <si>
-    <t>احسان</t>
-  </si>
-  <si>
-    <t>شاه‌ پروری</t>
-  </si>
-  <si>
-    <t>الکترونیک</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>هماهنگی و تماس صوتی با تلفن همراه یا تماس از طریق واتساپ از طریق شماره 09377988277</t>
-  </si>
-  <si>
-    <t>http://s11.picofile.com/file/8392736768/shahparvari.JPG</t>
-  </si>
-  <si>
-    <t>تاجیک</t>
-  </si>
-  <si>
-    <t>108</t>
-  </si>
-  <si>
-    <t>http://s11.picofile.com/file/8392736776/tajik.JPG</t>
-  </si>
-  <si>
-    <t>وحید</t>
-  </si>
-  <si>
-    <t>حاجی حسنی</t>
-  </si>
-  <si>
-    <t>109</t>
-  </si>
-  <si>
-    <t>هماهنگی و تماس با شماره همراه 09384220698 یا از طریق پیام رسان تلگرام و آیدی @Vahid_Hajihasani</t>
-  </si>
-  <si>
-    <t>http://s10.picofile.com/file/8392741726/HajiHasani.JPG</t>
   </si>
 </sst>
 </file>
@@ -954,54 +593,22 @@
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>26</v>
-      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
@@ -1028,24 +635,12 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="13">
-        <v>1</v>
-      </c>
-      <c r="L4" s="13">
-        <v>1</v>
-      </c>
-      <c r="M4" s="13">
-        <v>1</v>
-      </c>
-      <c r="N4" s="13">
-        <v>1</v>
-      </c>
-      <c r="O4" s="13">
-        <v>1</v>
-      </c>
-      <c r="P4" s="13">
-        <v>1</v>
-      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
@@ -1066,39 +661,17 @@
       <c r="A5" s="8">
         <v>2</v>
       </c>
-      <c r="B5" s="9">
-        <v>2</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
@@ -1156,45 +729,19 @@
       <c r="A7" s="8">
         <v>3</v>
       </c>
-      <c r="B7" s="14">
-        <v>3</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>45</v>
-      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
@@ -1250,39 +797,17 @@
       <c r="A9" s="8">
         <v>4</v>
       </c>
-      <c r="B9" s="14">
-        <v>4</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>52</v>
-      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
@@ -1315,9 +840,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="13"/>
-      <c r="L10" s="13">
-        <v>2</v>
-      </c>
+      <c r="L10" s="13"/>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
@@ -1342,30 +865,14 @@
       <c r="A11" s="8">
         <v>5</v>
       </c>
-      <c r="B11" s="14">
-        <v>5</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>57</v>
-      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
@@ -1426,30 +933,14 @@
       <c r="A13" s="8">
         <v>6</v>
       </c>
-      <c r="B13" s="14">
-        <v>6</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>64</v>
-      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
@@ -1510,30 +1001,14 @@
       <c r="A15" s="8">
         <v>7</v>
       </c>
-      <c r="B15" s="14">
-        <v>7</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>70</v>
-      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
@@ -1594,30 +1069,14 @@
       <c r="A17" s="8">
         <v>8</v>
       </c>
-      <c r="B17" s="14">
-        <v>8</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>74</v>
-      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
@@ -1678,30 +1137,14 @@
       <c r="A19" s="8">
         <v>9</v>
       </c>
-      <c r="B19" s="14">
-        <v>9</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>78</v>
-      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
@@ -1762,30 +1205,14 @@
       <c r="A21" s="8">
         <v>10</v>
       </c>
-      <c r="B21" s="14">
-        <v>10</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>84</v>
-      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
@@ -1846,30 +1273,14 @@
       <c r="A23" s="8">
         <v>11</v>
       </c>
-      <c r="B23" s="14">
-        <v>11</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>88</v>
-      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
@@ -1930,30 +1341,14 @@
       <c r="A25" s="8">
         <v>12</v>
       </c>
-      <c r="B25" s="14">
-        <v>12</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>92</v>
-      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
@@ -2014,30 +1409,14 @@
       <c r="A27" s="8">
         <v>13</v>
       </c>
-      <c r="B27" s="14">
-        <v>13</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>96</v>
-      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
@@ -2098,30 +1477,14 @@
       <c r="A29" s="8">
         <v>14</v>
       </c>
-      <c r="B29" s="14">
-        <v>14</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>100</v>
-      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
@@ -2182,30 +1545,14 @@
       <c r="A31" s="8">
         <v>15</v>
       </c>
-      <c r="B31" s="14">
-        <v>15</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>105</v>
-      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
@@ -2266,30 +1613,14 @@
       <c r="A33" s="8">
         <v>16</v>
       </c>
-      <c r="B33" s="14">
-        <v>16</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>110</v>
-      </c>
+      <c r="B33" s="14"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
@@ -2350,30 +1681,14 @@
       <c r="A35" s="8">
         <v>17</v>
       </c>
-      <c r="B35" s="14">
-        <v>17</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>115</v>
-      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
@@ -2434,30 +1749,14 @@
       <c r="A37" s="8">
         <v>18</v>
       </c>
-      <c r="B37" s="14">
-        <v>18</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>120</v>
-      </c>
+      <c r="B37" s="14"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
@@ -2518,30 +1817,14 @@
       <c r="A39" s="8">
         <v>19</v>
       </c>
-      <c r="B39" s="14">
-        <v>19</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I39" s="8" t="s">
-        <v>123</v>
-      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
       <c r="J39" s="8"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
@@ -2602,30 +1885,14 @@
       <c r="A41" s="8">
         <v>20</v>
       </c>
-      <c r="B41" s="14">
-        <v>20</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="I41" s="8" t="s">
-        <v>129</v>
-      </c>
+      <c r="B41" s="14"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
@@ -2686,30 +1953,14 @@
       <c r="A43" s="8">
         <v>21</v>
       </c>
-      <c r="B43" s="14">
-        <v>21</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I43" s="8" t="s">
-        <v>132</v>
-      </c>
+      <c r="B43" s="14"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
       <c r="J43" s="8"/>
       <c r="K43" s="13"/>
       <c r="L43" s="13"/>
@@ -2770,30 +2021,14 @@
       <c r="A45" s="8">
         <v>22</v>
       </c>
-      <c r="B45" s="14">
-        <v>22</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="I45" s="8" t="s">
-        <v>137</v>
-      </c>
+      <c r="B45" s="14"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
       <c r="J45" s="8"/>
       <c r="K45" s="13"/>
       <c r="L45" s="13"/>

</xml_diff>

<commit_message>
craete auto generator password for teachers enter code
</commit_message>
<xml_diff>
--- a/data/lastVersion.xlsx
+++ b/data/lastVersion.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="122">
   <si>
     <t>شماره ردیف</t>
   </si>
@@ -65,6 +65,319 @@
   </si>
   <si>
     <t>آیا این زمان تکمیل شده است؟</t>
+  </si>
+  <si>
+    <t>علیرضا</t>
+  </si>
+  <si>
+    <t>باقری</t>
+  </si>
+  <si>
+    <t>مهندسی برق</t>
+  </si>
+  <si>
+    <t>قدرت</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>برای هماهنگی قطعی شدن زمان به ایمیل alireza.bagheri.sh@gmail.com پیام بدهید.</t>
+  </si>
+  <si>
+    <t>http://uplod.ir/1u2rkn6hpaka/ali_bagheri.JPG.htm</t>
+  </si>
+  <si>
+    <t>شنبه ها بعد از ظهر</t>
+  </si>
+  <si>
+    <t>محمد</t>
+  </si>
+  <si>
+    <t>فتحی</t>
+  </si>
+  <si>
+    <t>مهندسی مکانیک</t>
+  </si>
+  <si>
+    <t>تبدیل انرژی</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>http://s11.picofile.com/file/8392736500/fathi.JPG</t>
+  </si>
+  <si>
+    <t>شنبه ها</t>
+  </si>
+  <si>
+    <t>دوشنب ها</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مصطفی </t>
+  </si>
+  <si>
+    <t>الوندیان</t>
+  </si>
+  <si>
+    <t>مخابرات</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>هماهنگی و تماس از طریق واتساپ و با 09212405364</t>
+  </si>
+  <si>
+    <t>http://s10.picofile.com/file/8392736442/alvandian.JPG</t>
+  </si>
+  <si>
+    <t>یک شنبه ساعت 5 تا 8</t>
+  </si>
+  <si>
+    <t>دوشنبه</t>
+  </si>
+  <si>
+    <t>دوشنبه ساعت 6</t>
+  </si>
+  <si>
+    <t>سه شنبه</t>
+  </si>
+  <si>
+    <t>ایوب</t>
+  </si>
+  <si>
+    <t>حسنی</t>
+  </si>
+  <si>
+    <t>طراحی کاربردی</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>http://s10.picofile.com/file/8392736450/ayoub_hasani.JPG</t>
+  </si>
+  <si>
+    <t>شنبه</t>
+  </si>
+  <si>
+    <t>یکشنبه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">علیرضا </t>
+  </si>
+  <si>
+    <t>قادری</t>
+  </si>
+  <si>
+    <t>مهندسی نفت</t>
+  </si>
+  <si>
+    <t>مخازن هیدروکربوری</t>
+  </si>
+  <si>
+    <t>701</t>
+  </si>
+  <si>
+    <t>http://s10.picofile.com/file/8392736526/ghaderi.JPG</t>
+  </si>
+  <si>
+    <t>محسن</t>
+  </si>
+  <si>
+    <t>غلامی</t>
+  </si>
+  <si>
+    <t>204</t>
+  </si>
+  <si>
+    <t>http://s11.picofile.com/file/8392736550/gholami.JPG</t>
+  </si>
+  <si>
+    <t>رمضان</t>
+  </si>
+  <si>
+    <t>حسینی</t>
+  </si>
+  <si>
+    <t>205</t>
+  </si>
+  <si>
+    <t>http://s11.picofile.com/file/8392736592/hoseini.JPG</t>
+  </si>
+  <si>
+    <t>سعید</t>
+  </si>
+  <si>
+    <t>جلیلوند</t>
+  </si>
+  <si>
+    <t>206</t>
+  </si>
+  <si>
+    <t>http://s11.picofile.com/file/8392736626/jalilvand.JPG</t>
+  </si>
+  <si>
+    <t>سیدحسین</t>
+  </si>
+  <si>
+    <t>کمالی</t>
+  </si>
+  <si>
+    <t>207</t>
+  </si>
+  <si>
+    <t>http://s11.picofile.com/file/8392741392/kamali.JPG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">محمدرضا </t>
+  </si>
+  <si>
+    <t>فرحناک</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>http://s11.picofile.com/file/8392736484/farahnak.JPG</t>
+  </si>
+  <si>
+    <t>جمال</t>
+  </si>
+  <si>
+    <t>کزازی</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>تماس از طریق تلفن یا تلگرام با شماره 9187042184</t>
+  </si>
+  <si>
+    <t>http://s10.picofile.com/file/8392736976/kazzazi.JPG</t>
+  </si>
+  <si>
+    <t>کورش</t>
+  </si>
+  <si>
+    <t>خلج مفرد</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">هماهنگی و تماس از طریق تلگرام با ایدی @Kkmonfared و همچنین تماس از طریق اسکایپ با شماره 9128303218
+</t>
+  </si>
+  <si>
+    <t>http://s10.picofile.com/file/8392736684/khalaj.JPG</t>
+  </si>
+  <si>
+    <t>سیدمیلاد</t>
+  </si>
+  <si>
+    <t>میری</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>هماهنگی و تماس صوتی با تلفن همراه یا تماس از طریق واتساپ از طریق شماره 09117716042</t>
+  </si>
+  <si>
+    <t>http://s11.picofile.com/file/8392736718/miri.JPG</t>
+  </si>
+  <si>
+    <t>امیر</t>
+  </si>
+  <si>
+    <t>ملایی</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>هماهنگی و تماس با تلفن همراه از طریق شماره 9157131289</t>
+  </si>
+  <si>
+    <t>http://s10.picofile.com/file/8392736726/mollaii.JPG</t>
+  </si>
+  <si>
+    <t>حسین</t>
+  </si>
+  <si>
+    <t>208</t>
+  </si>
+  <si>
+    <t>http://s11.picofile.com/file/8392736742/saeed_hosein.JPG</t>
+  </si>
+  <si>
+    <t>احسان</t>
+  </si>
+  <si>
+    <t>شاه‌ پروری</t>
+  </si>
+  <si>
+    <t>الکترونیک</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>هماهنگی و تماس صوتی با تلفن همراه یا تماس از طریق واتساپ از طریق شماره 09377988277</t>
+  </si>
+  <si>
+    <t>http://s11.picofile.com/file/8392736768/shahparvari.JPG</t>
+  </si>
+  <si>
+    <t>علی</t>
+  </si>
+  <si>
+    <t>تاجیک</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>http://s11.picofile.com/file/8392736776/tajik.JPG</t>
+  </si>
+  <si>
+    <t>وحید</t>
+  </si>
+  <si>
+    <t>حاجی حسنی</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>هماهنگی و تماس با شماره همراه 09384220698 یا از طریق پیام رسان تلگرام و آیدی @Vahid_Hajihasani</t>
+  </si>
+  <si>
+    <t>http://s10.picofile.com/file/8392741726/HajiHasani.JPG</t>
+  </si>
+  <si>
+    <t>اکبر</t>
+  </si>
+  <si>
+    <t>یوسفی</t>
+  </si>
+  <si>
+    <t>aVAIwJ4GH2</t>
+  </si>
+  <si>
+    <t>@golam</t>
+  </si>
+  <si>
+    <t>https://ece.ut.ac.ir/image/edu/teacher?img_id=71874335&amp;t=1585488639782</t>
+  </si>
+  <si>
+    <t>پسر خوبیه هستند</t>
   </si>
 </sst>
 </file>
@@ -593,22 +906,52 @@
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
+      <c r="K3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>25</v>
+      </c>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
@@ -635,12 +978,24 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
+      <c r="K4" s="13">
+        <v>1</v>
+      </c>
+      <c r="L4" s="13">
+        <v>1</v>
+      </c>
+      <c r="M4" s="13">
+        <v>1</v>
+      </c>
+      <c r="N4" s="13">
+        <v>1</v>
+      </c>
+      <c r="O4" s="13">
+        <v>1</v>
+      </c>
+      <c r="P4" s="13">
+        <v>1</v>
+      </c>
       <c r="Q4" s="13"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
@@ -661,17 +1016,37 @@
       <c r="A5" s="8">
         <v>2</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+      <c r="B5" s="9">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="J5" s="11"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
+      <c r="K5" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>34</v>
+      </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
@@ -729,19 +1104,43 @@
       <c r="A7" s="8">
         <v>3</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="B7" s="14">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="J7" s="8"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
+      <c r="K7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
@@ -797,17 +1196,37 @@
       <c r="A9" s="8">
         <v>4</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="B9" s="14">
+        <v>4</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="J9" s="8"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="K9" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
@@ -840,7 +1259,9 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+      <c r="L10" s="13">
+        <v>2</v>
+      </c>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
@@ -865,14 +1286,30 @@
       <c r="A11" s="8">
         <v>5</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="B11" s="14">
+        <v>5</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="J11" s="8"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
@@ -933,14 +1370,30 @@
       <c r="A13" s="8">
         <v>6</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="B13" s="14">
+        <v>6</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="J13" s="8"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
@@ -1001,14 +1454,30 @@
       <c r="A15" s="8">
         <v>7</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
+      <c r="B15" s="14">
+        <v>7</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="J15" s="8"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
@@ -1069,14 +1538,30 @@
       <c r="A17" s="8">
         <v>8</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
+      <c r="B17" s="14">
+        <v>8</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="J17" s="8"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
@@ -1137,14 +1622,30 @@
       <c r="A19" s="8">
         <v>9</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
+      <c r="B19" s="14">
+        <v>9</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>73</v>
+      </c>
       <c r="J19" s="8"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
@@ -1205,14 +1706,30 @@
       <c r="A21" s="8">
         <v>10</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="B21" s="14">
+        <v>10</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>77</v>
+      </c>
       <c r="J21" s="8"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
@@ -1273,14 +1790,30 @@
       <c r="A23" s="8">
         <v>11</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="B23" s="14">
+        <v>11</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="J23" s="8"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
@@ -1341,14 +1874,30 @@
       <c r="A25" s="8">
         <v>12</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
+      <c r="B25" s="14">
+        <v>12</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="J25" s="8"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
@@ -1409,14 +1958,30 @@
       <c r="A27" s="8">
         <v>13</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
+      <c r="B27" s="14">
+        <v>13</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="J27" s="8"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
@@ -1477,14 +2042,30 @@
       <c r="A29" s="8">
         <v>14</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
+      <c r="B29" s="14">
+        <v>14</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="J29" s="8"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
@@ -1545,14 +2126,30 @@
       <c r="A31" s="8">
         <v>15</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
+      <c r="B31" s="14">
+        <v>15</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="J31" s="8"/>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
@@ -1613,14 +2210,30 @@
       <c r="A33" s="8">
         <v>16</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
+      <c r="B33" s="14">
+        <v>16</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>106</v>
+      </c>
       <c r="J33" s="8"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
@@ -1681,14 +2294,30 @@
       <c r="A35" s="8">
         <v>17</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+      <c r="B35" s="14">
+        <v>17</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>110</v>
+      </c>
       <c r="J35" s="8"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
@@ -1749,14 +2378,30 @@
       <c r="A37" s="8">
         <v>18</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
+      <c r="B37" s="14">
+        <v>18</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>115</v>
+      </c>
       <c r="J37" s="8"/>
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
@@ -1817,16 +2462,36 @@
       <c r="A39" s="8">
         <v>19</v>
       </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="13"/>
+      <c r="B39" s="14">
+        <v>19</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="K39" s="13" t="s">
+        <v>25</v>
+      </c>
       <c r="L39" s="13"/>
       <c r="M39" s="13"/>
       <c r="N39" s="13"/>

</xml_diff>

<commit_message>
fix reading excel timeslots
</commit_message>
<xml_diff>
--- a/data/lastVersion.xlsx
+++ b/data/lastVersion.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="195">
   <si>
     <t>شماره ردیف</t>
   </si>
@@ -79,16 +79,22 @@
     <t>قدرت</t>
   </si>
   <si>
-    <t>101</t>
+    <t>fRQRQqEYjq</t>
   </si>
   <si>
     <t>برای هماهنگی قطعی شدن زمان به ایمیل alireza.bagheri.sh@gmail.com پیام بدهید.</t>
   </si>
   <si>
-    <t>http://uplod.ir/1u2rkn6hpaka/ali_bagheri.JPG.htm</t>
+    <t>http://s11.picofile.com/file/8392736434/ali_bagheri.JPG</t>
   </si>
   <si>
-    <t>شنبه ها بعد از ظهر</t>
+    <t>مهندسی برق - قدرت</t>
+  </si>
+  <si>
+    <t>22 فروردین ماه، ساعت 11</t>
+  </si>
+  <si>
+    <t>22 فروردین ماه، ساعت 17</t>
   </si>
   <si>
     <t>محمد</t>
@@ -103,70 +109,25 @@
     <t>تبدیل انرژی</t>
   </si>
   <si>
-    <t>201</t>
+    <t>WREN2z4tr4</t>
   </si>
   <si>
-    <t>N</t>
+    <t>هماهنگی و تماس از طریق شماره تماس 09379411263</t>
   </si>
   <si>
     <t>http://s11.picofile.com/file/8392736500/fathi.JPG</t>
   </si>
   <si>
-    <t>شنبه ها</t>
+    <t>مهندسی مکانیک - تبدیل انرژی</t>
   </si>
   <si>
-    <t>دوشنب ها</t>
+    <t>18 فروردین. ساعت 17-18:30</t>
   </si>
   <si>
-    <t xml:space="preserve">مصطفی </t>
+    <t xml:space="preserve"> 19 فروردین. ساعت 17-18:30</t>
   </si>
   <si>
-    <t>الوندیان</t>
-  </si>
-  <si>
-    <t>مخابرات</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>هماهنگی و تماس از طریق واتساپ و با 09212405364</t>
-  </si>
-  <si>
-    <t>http://s10.picofile.com/file/8392736442/alvandian.JPG</t>
-  </si>
-  <si>
-    <t>یک شنبه ساعت 5 تا 8</t>
-  </si>
-  <si>
-    <t>دوشنبه</t>
-  </si>
-  <si>
-    <t>دوشنبه ساعت 6</t>
-  </si>
-  <si>
-    <t>سه شنبه</t>
-  </si>
-  <si>
-    <t>ایوب</t>
-  </si>
-  <si>
-    <t>حسنی</t>
-  </si>
-  <si>
-    <t>طراحی کاربردی</t>
-  </si>
-  <si>
-    <t>202</t>
-  </si>
-  <si>
-    <t>http://s10.picofile.com/file/8392736450/ayoub_hasani.JPG</t>
-  </si>
-  <si>
-    <t>شنبه</t>
-  </si>
-  <si>
-    <t>یکشنبه</t>
+    <t xml:space="preserve"> 20 فروردین. ساعت 17-18:30</t>
   </si>
   <si>
     <t xml:space="preserve">علیرضا </t>
@@ -181,10 +142,110 @@
     <t>مخازن هیدروکربوری</t>
   </si>
   <si>
-    <t>701</t>
+    <t>rUQzIoy67R</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
   <si>
     <t>http://s10.picofile.com/file/8392736526/ghaderi.JPG</t>
+  </si>
+  <si>
+    <t>مهندسی نفت - مخازن هیدروکربوری</t>
+  </si>
+  <si>
+    <t>18 فروردین ساعت 18 تا 19</t>
+  </si>
+  <si>
+    <t>19 فروردین ساعت 18 تا 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">محمدرضا </t>
+  </si>
+  <si>
+    <t>فرحناک</t>
+  </si>
+  <si>
+    <t>طراحی کاربردی</t>
+  </si>
+  <si>
+    <t>yVT5bzwdtk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">هماهنگی تماس از طریق ایدی تلگرامی @Mreza_farahnak
+</t>
+  </si>
+  <si>
+    <t>http://s11.picofile.com/file/8392736484/farahnak.JPG</t>
+  </si>
+  <si>
+    <t>مهندسی مکانیک - طراحی کاربردی</t>
+  </si>
+  <si>
+    <t>18 فروردین. ساعت 18-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19 فروردین. ساعت 18-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20 فروردین. ساعت 18-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مصطفی </t>
+  </si>
+  <si>
+    <t>الوندیان</t>
+  </si>
+  <si>
+    <t>مخابرات</t>
+  </si>
+  <si>
+    <t>TjsUjDatfS</t>
+  </si>
+  <si>
+    <t>هماهنگی و تماس از طریق واتساپ و با 09212405364</t>
+  </si>
+  <si>
+    <t>http://s10.picofile.com/file/8392736442/alvandian.JPG</t>
+  </si>
+  <si>
+    <t>مهندسی برق - مخابرات</t>
+  </si>
+  <si>
+    <t>19 فروردین ساعت 16 تا 19</t>
+  </si>
+  <si>
+    <t>20 فروردین ساعت 10 تا 12</t>
+  </si>
+  <si>
+    <t>۲۰ فروردین ساعت 16 تا 19</t>
+  </si>
+  <si>
+    <t>ایوب</t>
+  </si>
+  <si>
+    <t>حسنی</t>
+  </si>
+  <si>
+    <t>GPq3HM3THE</t>
+  </si>
+  <si>
+    <t>http://s10.picofile.com/file/8392736450/ayoub_hasani.JPG</t>
+  </si>
+  <si>
+    <t>16 فروردین ساعت 18 تا 19</t>
+  </si>
+  <si>
+    <t>17 فروردین ساعت 18 تا 19</t>
+  </si>
+  <si>
+    <t>20 فروردین ساعت 18 تا 19</t>
+  </si>
+  <si>
+    <t>21 فروردین ساعت 18 تا 19</t>
+  </si>
+  <si>
+    <t>22 فروردین ساعت 18 تا 19</t>
   </si>
   <si>
     <t>محسن</t>
@@ -193,10 +254,22 @@
     <t>غلامی</t>
   </si>
   <si>
-    <t>204</t>
+    <t>dXoGRhNRYt</t>
+  </si>
+  <si>
+    <t>هماهنگی تماس از طریق ایدی تلگرامی @MsnGhmi</t>
   </si>
   <si>
     <t>http://s11.picofile.com/file/8392736550/gholami.JPG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18 فروردین. 8-10 (به وقت ایران)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19 فروردین. 8-10 (به وقت ایران)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20 فروردین. 8-10 (به وقت ایران)</t>
   </si>
   <si>
     <t>رمضان</t>
@@ -205,10 +278,19 @@
     <t>حسینی</t>
   </si>
   <si>
-    <t>205</t>
+    <t>ml6HHB3vyc</t>
   </si>
   <si>
     <t>http://s11.picofile.com/file/8392736592/hoseini.JPG</t>
+  </si>
+  <si>
+    <t>18 فروردین ساعت 20 تا 12</t>
+  </si>
+  <si>
+    <t>19 فروردین ساعت 20 تا 12</t>
+  </si>
+  <si>
+    <t>20 فروردین ساعت 20 تا 12</t>
   </si>
   <si>
     <t>سعید</t>
@@ -217,10 +299,34 @@
     <t>جلیلوند</t>
   </si>
   <si>
-    <t>206</t>
+    <t>2OQs50FBCo</t>
   </si>
   <si>
     <t>http://s11.picofile.com/file/8392736626/jalilvand.JPG</t>
+  </si>
+  <si>
+    <t>16 فروردین ساعت 9-10</t>
+  </si>
+  <si>
+    <t>17 فروردین ساعت 17 تا 16</t>
+  </si>
+  <si>
+    <t>18 فروردین ساعت 9-10</t>
+  </si>
+  <si>
+    <t>19 فروردین ساعت 17 تا 16</t>
+  </si>
+  <si>
+    <t>20 فروردین ساعت 9-10</t>
+  </si>
+  <si>
+    <t>21 فروردین ساعت 17 تا 16</t>
+  </si>
+  <si>
+    <t>22 فروردین ساعت 9-10</t>
+  </si>
+  <si>
+    <t>22 فروردین ساعت 17 تا 16</t>
   </si>
   <si>
     <t>سیدحسین</t>
@@ -229,22 +335,19 @@
     <t>کمالی</t>
   </si>
   <si>
-    <t>207</t>
+    <t>hoJTL3Og7Y</t>
   </si>
   <si>
     <t>http://s11.picofile.com/file/8392741392/kamali.JPG</t>
   </si>
   <si>
-    <t xml:space="preserve">محمدرضا </t>
+    <t>18 فروردین، یک ساعت توافقی</t>
   </si>
   <si>
-    <t>فرحناک</t>
+    <t>19 فروردین، یک ساعت توافقی</t>
   </si>
   <si>
-    <t>203</t>
-  </si>
-  <si>
-    <t>http://s11.picofile.com/file/8392736484/farahnak.JPG</t>
+    <t>20 فروردین، یک ساعت توافقی</t>
   </si>
   <si>
     <t>جمال</t>
@@ -253,7 +356,7 @@
     <t>کزازی</t>
   </si>
   <si>
-    <t>103</t>
+    <t>9M0zXoQdqh</t>
   </si>
   <si>
     <t>تماس از طریق تلفن یا تلگرام با شماره 9187042184</t>
@@ -262,13 +365,22 @@
     <t>http://s10.picofile.com/file/8392736976/kazzazi.JPG</t>
   </si>
   <si>
+    <t>18 فروردین. ساعت 17-20</t>
+  </si>
+  <si>
+    <t>19 فروردین. ساعت 18-20</t>
+  </si>
+  <si>
+    <t>20 فروردین. ساعت 16-19</t>
+  </si>
+  <si>
     <t>کورش</t>
   </si>
   <si>
     <t>خلج مفرد</t>
   </si>
   <si>
-    <t>104</t>
+    <t>u37VMTksrf</t>
   </si>
   <si>
     <t xml:space="preserve">هماهنگی و تماس از طریق تلگرام با ایدی @Kkmonfared و همچنین تماس از طریق اسکایپ با شماره 9128303218
@@ -278,13 +390,19 @@
     <t>http://s10.picofile.com/file/8392736684/khalaj.JPG</t>
   </si>
   <si>
+    <t>21 فروردین. ساعت 14-15</t>
+  </si>
+  <si>
+    <t>22 فروردین. ساعت 14-15</t>
+  </si>
+  <si>
     <t>سیدمیلاد</t>
   </si>
   <si>
     <t>میری</t>
   </si>
   <si>
-    <t>105</t>
+    <t>wDAk68R3QR</t>
   </si>
   <si>
     <t>هماهنگی و تماس صوتی با تلفن همراه یا تماس از طریق واتساپ از طریق شماره 09117716042</t>
@@ -293,13 +411,22 @@
     <t>http://s11.picofile.com/file/8392736718/miri.JPG</t>
   </si>
   <si>
+    <t>18 فروردین. ساعت 18-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19 فروردین. ساعت 18-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20 فروردین. ساعت 18-11</t>
+  </si>
+  <si>
     <t>امیر</t>
   </si>
   <si>
     <t>ملایی</t>
   </si>
   <si>
-    <t>106</t>
+    <t>OAE9mBtufq</t>
   </si>
   <si>
     <t>هماهنگی و تماس با تلفن همراه از طریق شماره 9157131289</t>
@@ -308,13 +435,34 @@
     <t>http://s10.picofile.com/file/8392736726/mollaii.JPG</t>
   </si>
   <si>
+    <t>18 فروردین. ساعت 18-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19 فروردین. ساعت 18-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20 فروردین. ساعت 18-16</t>
+  </si>
+  <si>
     <t>حسین</t>
   </si>
   <si>
-    <t>208</t>
+    <t>BgCVEyc7oL</t>
+  </si>
+  <si>
+    <t>هماهنگی و تماس از طریق شماره تماس 09122508337</t>
   </si>
   <si>
     <t>http://s11.picofile.com/file/8392736742/saeed_hosein.JPG</t>
+  </si>
+  <si>
+    <t>18 فروردین ساعت 19:30 تا 19</t>
+  </si>
+  <si>
+    <t>19 فروردین ساعت 19:30 تا 19</t>
+  </si>
+  <si>
+    <t>20 فروردین ساعت 19:30 تا 19</t>
   </si>
   <si>
     <t>احسان</t>
@@ -326,7 +474,7 @@
     <t>الکترونیک</t>
   </si>
   <si>
-    <t>107</t>
+    <t>RpRxaU1Tnv</t>
   </si>
   <si>
     <t>هماهنگی و تماس صوتی با تلفن همراه یا تماس از طریق واتساپ از طریق شماره 09377988277</t>
@@ -335,13 +483,27 @@
     <t>http://s11.picofile.com/file/8392736768/shahparvari.JPG</t>
   </si>
   <si>
+    <t>مهندسی برق - الکترونیک</t>
+  </si>
+  <si>
+    <t>18 فروردین ساعت 16 تا 19</t>
+  </si>
+  <si>
+    <t>20 فروردین ساعت 16 تا 19</t>
+  </si>
+  <si>
     <t>علی</t>
   </si>
   <si>
     <t>تاجیک</t>
   </si>
   <si>
-    <t>108</t>
+    <t>mlKF9VydGX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تماس با تلفن همراه یا تماس صوتی با واتساپ
+با شماره: 09127717602
+ترجیح با تماس به شماره تلفن همراه</t>
   </si>
   <si>
     <t>http://s11.picofile.com/file/8392736776/tajik.JPG</t>
@@ -353,7 +515,7 @@
     <t>حاجی حسنی</t>
   </si>
   <si>
-    <t>109</t>
+    <t>Bg7kK7M1gk</t>
   </si>
   <si>
     <t>هماهنگی و تماس با شماره همراه 09384220698 یا از طریق پیام رسان تلگرام و آیدی @Vahid_Hajihasani</t>
@@ -362,22 +524,84 @@
     <t>http://s10.picofile.com/file/8392741726/HajiHasani.JPG</t>
   </si>
   <si>
-    <t>اکبر</t>
+    <t>18 فروردین. ساعت 22-21</t>
   </si>
   <si>
-    <t>یوسفی</t>
+    <t xml:space="preserve"> 19 فروردین. ساعت 22-21</t>
   </si>
   <si>
-    <t>aVAIwJ4GH2</t>
+    <t xml:space="preserve"> 20 فروردین. ساعت 22-21</t>
   </si>
   <si>
-    <t>@golam</t>
+    <t>خوش اخلاق</t>
   </si>
   <si>
-    <t>https://ece.ut.ac.ir/image/edu/teacher?img_id=71874335&amp;t=1585488639782</t>
+    <t>9dhCcoDWmE</t>
   </si>
   <si>
-    <t>پسر خوبیه هستند</t>
+    <t xml:space="preserve">هماهنگی تماس از طریق ارسال پیام در تلگرام با ایدی @DrKhoshakhlagh یا واتساپ روی شماره 09124880702
+</t>
+  </si>
+  <si>
+    <t>http://s10.picofile.com/file/8392878418/khoshakhlagh.JPG</t>
+  </si>
+  <si>
+    <t>هجده فروردین. نیم ساعت توافقی</t>
+  </si>
+  <si>
+    <t>نوزده فروردین. نیم ساعت توافقی</t>
+  </si>
+  <si>
+    <t>بیست فروردین. نیم ساعت توافقی</t>
+  </si>
+  <si>
+    <t>حامد</t>
+  </si>
+  <si>
+    <t>عالمی</t>
+  </si>
+  <si>
+    <t>Qi64Z9lRPP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">هماهنگی و تماس از طریق شماره همراه 09109339615
+</t>
+  </si>
+  <si>
+    <t>http://s10.picofile.com/file/8392878350/alemi.JPG</t>
+  </si>
+  <si>
+    <t>18 فروردین. ساعت 18-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20 فروردین. ساعت 18-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19 فروردین. ساعت 18-17</t>
+  </si>
+  <si>
+    <t>محمدمتین</t>
+  </si>
+  <si>
+    <t>بهزادی</t>
+  </si>
+  <si>
+    <t>dqtWHhmN2l</t>
+  </si>
+  <si>
+    <t>هماهنگی و تماس از طریق تماس تلفنی یا پیامک از طریق شماره همراه 09198958869</t>
+  </si>
+  <si>
+    <t>http://s11.picofile.com/file/8392878392/behzadi.JPG</t>
+  </si>
+  <si>
+    <t>نوزده فروردین 20-20:30</t>
+  </si>
+  <si>
+    <t>هجده فروردین 20-20:30</t>
+  </si>
+  <si>
+    <t>بیست فروردین 20-20:30</t>
   </si>
 </sst>
 </file>
@@ -930,28 +1154,20 @@
       <c r="I3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>25</v>
       </c>
+      <c r="K3" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="L3" s="12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
-      <c r="M3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>25</v>
-      </c>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
@@ -978,24 +1194,12 @@
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="13">
-        <v>1</v>
-      </c>
-      <c r="L4" s="13">
-        <v>1</v>
-      </c>
-      <c r="M4" s="13">
-        <v>1</v>
-      </c>
-      <c r="N4" s="13">
-        <v>1</v>
-      </c>
-      <c r="O4" s="13">
-        <v>1</v>
-      </c>
-      <c r="P4" s="13">
-        <v>1</v>
-      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
@@ -1020,34 +1224,38 @@
         <v>2</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
-      <c r="J5" s="11"/>
+      <c r="J5" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="K5" s="13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
-      <c r="M5" s="13"/>
+      <c r="M5" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
@@ -1108,39 +1316,37 @@
         <v>3</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
-      <c r="J7" s="8"/>
+      <c r="J7" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="K7" s="13" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
-      <c r="M7" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>44</v>
-      </c>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
@@ -1200,34 +1406,38 @@
         <v>4</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
-      <c r="J9" s="8"/>
+      <c r="J9" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="K9" s="13" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
-      <c r="M9" s="13"/>
+      <c r="M9" s="13" t="s">
+        <v>58</v>
+      </c>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
@@ -1259,9 +1469,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="13"/>
-      <c r="L10" s="13">
-        <v>2</v>
-      </c>
+      <c r="L10" s="13"/>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
       <c r="O10" s="13"/>
@@ -1290,30 +1498,38 @@
         <v>5</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
+      <c r="J11" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
@@ -1374,34 +1590,50 @@
         <v>6</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F13" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="M13" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>60</v>
+      <c r="N13" s="13" t="s">
+        <v>48</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>31</v>
+      <c r="O13" s="13" t="s">
+        <v>75</v>
       </c>
-      <c r="I13" s="8" t="s">
-        <v>61</v>
+      <c r="P13" s="13" t="s">
+        <v>76</v>
       </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
+      <c r="Q13" s="13" t="s">
+        <v>77</v>
+      </c>
       <c r="R13" s="7"/>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
@@ -1458,30 +1690,38 @@
         <v>7</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
-      <c r="J15" s="8"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
+      <c r="J15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
       <c r="P15" s="13"/>
@@ -1542,30 +1782,38 @@
         <v>8</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
+      <c r="J17" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>92</v>
+      </c>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
       <c r="P17" s="13"/>
@@ -1626,35 +1874,53 @@
         <v>9</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
-      <c r="J19" s="8"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="7"/>
+      <c r="J19" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="N19" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="O19" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="P19" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q19" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
@@ -1710,30 +1976,38 @@
         <v>10</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
+      <c r="J21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>111</v>
+      </c>
       <c r="N21" s="13"/>
       <c r="O21" s="13"/>
       <c r="P21" s="13"/>
@@ -1794,30 +2068,38 @@
         <v>11</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>20</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
-      <c r="J23" s="8"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
+      <c r="J23" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>119</v>
+      </c>
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
       <c r="P23" s="13"/>
@@ -1878,10 +2160,10 @@
         <v>12</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>20</v>
@@ -1890,17 +2172,23 @@
         <v>21</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
-      <c r="J25" s="8"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
+      <c r="J25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>126</v>
+      </c>
       <c r="M25" s="13"/>
       <c r="N25" s="13"/>
       <c r="O25" s="13"/>
@@ -1962,30 +2250,38 @@
         <v>13</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>20</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>90</v>
+        <v>129</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
-      <c r="J27" s="8"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
+      <c r="J27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="L27" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="M27" s="13" t="s">
+        <v>134</v>
+      </c>
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
       <c r="P27" s="13"/>
@@ -2046,30 +2342,38 @@
         <v>14</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>94</v>
+        <v>136</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>20</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>97</v>
+        <v>139</v>
       </c>
-      <c r="J29" s="8"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
+      <c r="J29" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="M29" s="13" t="s">
+        <v>142</v>
+      </c>
       <c r="N29" s="13"/>
       <c r="O29" s="13"/>
       <c r="P29" s="13"/>
@@ -2130,30 +2434,38 @@
         <v>15</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>100</v>
+        <v>146</v>
       </c>
-      <c r="J31" s="8"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
+      <c r="J31" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K31" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="M31" s="13" t="s">
+        <v>149</v>
+      </c>
       <c r="N31" s="13"/>
       <c r="O31" s="13"/>
       <c r="P31" s="13"/>
@@ -2214,30 +2526,38 @@
         <v>16</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>101</v>
+        <v>150</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
       <c r="E33" s="15" t="s">
         <v>20</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>104</v>
+        <v>153</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>105</v>
+        <v>154</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>106</v>
+        <v>155</v>
       </c>
-      <c r="J33" s="8"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
+      <c r="J33" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="L33" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="M33" s="13" t="s">
+        <v>158</v>
+      </c>
       <c r="N33" s="13"/>
       <c r="O33" s="13"/>
       <c r="P33" s="13"/>
@@ -2298,30 +2618,38 @@
         <v>17</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>107</v>
+        <v>159</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="E35" s="15" t="s">
         <v>20</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>109</v>
+        <v>161</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>110</v>
+        <v>163</v>
       </c>
-      <c r="J35" s="8"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
+      <c r="J35" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M35" s="13" t="s">
+        <v>158</v>
+      </c>
       <c r="N35" s="13"/>
       <c r="O35" s="13"/>
       <c r="P35" s="13"/>
@@ -2382,10 +2710,10 @@
         <v>18</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>111</v>
+        <v>164</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>112</v>
+        <v>165</v>
       </c>
       <c r="E37" s="15" t="s">
         <v>20</v>
@@ -2394,18 +2722,26 @@
         <v>21</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>113</v>
+        <v>166</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>114</v>
+        <v>167</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>115</v>
+        <v>168</v>
       </c>
-      <c r="J37" s="8"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
+      <c r="J37" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="L37" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="M37" s="13" t="s">
+        <v>171</v>
+      </c>
       <c r="N37" s="13"/>
       <c r="O37" s="13"/>
       <c r="P37" s="13"/>
@@ -2466,34 +2802,38 @@
         <v>19</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>116</v>
+        <v>28</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>117</v>
+        <v>172</v>
       </c>
       <c r="E39" s="15" t="s">
         <v>20</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>21</v>
+        <v>152</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>118</v>
+        <v>173</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>119</v>
+        <v>174</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>120</v>
+        <v>175</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>121</v>
+        <v>156</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>25</v>
+        <v>176</v>
       </c>
-      <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
+      <c r="L39" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="M39" s="13" t="s">
+        <v>178</v>
+      </c>
       <c r="N39" s="13"/>
       <c r="O39" s="13"/>
       <c r="P39" s="13"/>
@@ -2550,18 +2890,42 @@
       <c r="A41" s="8">
         <v>20</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
+      <c r="B41" s="14">
+        <v>20</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="L41" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M41" s="13" t="s">
+        <v>186</v>
+      </c>
       <c r="N41" s="13"/>
       <c r="O41" s="13"/>
       <c r="P41" s="13"/>
@@ -2618,18 +2982,42 @@
       <c r="A43" s="8">
         <v>21</v>
       </c>
-      <c r="B43" s="14"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="13"/>
-      <c r="M43" s="13"/>
+      <c r="B43" s="14">
+        <v>21</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K43" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="L43" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="M43" s="13" t="s">
+        <v>194</v>
+      </c>
       <c r="N43" s="13"/>
       <c r="O43" s="13"/>
       <c r="P43" s="13"/>

</xml_diff>

<commit_message>
when new teahcer added then send message to student that have this teacher gerayesh
</commit_message>
<xml_diff>
--- a/data/lastVersion.xlsx
+++ b/data/lastVersion.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="197">
   <si>
     <t>شماره ردیف</t>
   </si>
@@ -606,6 +606,9 @@
   <si>
     <t>هجده فروردین 20-20:30</t>
   </si>
+  <si>
+    <t>Ag6KmwEAac</t>
+  </si>
 </sst>
 </file>
 
@@ -1198,7 +1201,9 @@
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="L4" s="13">
+        <v>1</v>
+      </c>
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
       <c r="O4" s="13"/>
@@ -3085,15 +3090,33 @@
       <c r="A45" s="8">
         <v>22</v>
       </c>
-      <c r="B45" s="14"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
+      <c r="B45" s="14">
+        <v>22</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="K45" s="13"/>
       <c r="L45" s="13"/>
       <c r="M45" s="13"/>

</xml_diff>